<commit_message>
greedy algorithm implemented in python
</commit_message>
<xml_diff>
--- a/place_data.xlsx
+++ b/place_data.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6cf1c5c7ee8f8e63/Desktop/Computer Science/Pune Food Tour/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_401D6AC0C750F5A143EECF314BCBC914315D2137" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3ADA63A4-2EF5-4285-A98A-81851FA829E8}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_9025CE2E861814395D8FEBBFA2A78E16F5298CD5" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A25AA744-0741-47F0-AF3B-903D17B3FC4B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="13" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -256,1732 +256,1732 @@
     <t>18.5278236</t>
   </si>
   <si>
-    <t>HOMEtoHOME</t>
-  </si>
-  <si>
-    <t>HOMEtoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>HOMEtoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>HOMEtoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>HOMEtoSujata Mastani</t>
-  </si>
-  <si>
-    <t>HOMEtoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>HOMEtoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>HOMEtoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>HOMEtoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>HOMEtoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>HOMEtoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>HOMEtoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>HOMEtoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>HOMEtoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>HOMEtoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>HOMEtoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>HOMEtoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>HOMEtoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>HOMEtoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>HOMEtoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>HOMEtoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>HOMEtoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>HOMEtoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>HOMEtoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoHOME</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Garden Vada PavtoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoHOME</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Santosh Bakery: PatticetoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoHOME</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Chitale Bandhu: BakarwaditoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoHOME</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Sujata MastanitoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoHOME</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Flavours Sandwich: Chocolate ToasttoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoHOME</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Rudra Café: BreadcrumbstoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoHOME</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Vaishali: Cold BournvitatoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoHOME</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Kayani Bakery: Shrewsbury CookiestoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoHOME</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Yewale Amruttulya: TeatoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoHOME</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Cafe Goodluck: Bun MaskatoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoHOME</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Falahaar: Jamun ShottoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoHOME</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Yashwant DabelitoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoHOME</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Durga Cafe: Cold Coffee and Anda BhurjitoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoHOME</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Sukanta: ThalitoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoHOME</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Kadhai: JalebitoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoHOME</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Indorilaal: KachoritoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoHOME</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Kohinoor Restaurant: Omelette and ChaitoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoHOME</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Kalyan Bhel: Pani PuritoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoHOME</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoSujata Mastani</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>The Place: SizzlertoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoHOME</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Jain Boarding: Lunch MenutoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoHOME</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Bhadait Misal: MisaltoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoHOME</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Masaledar Biryani House: BiryanitoShiv Kailash Dairy: Special Doodh</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoHOME</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoGarden Vada Pav</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoSantosh Bakery: Pattice</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoChitale Bandhu: Bakarwadi</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoSujata Mastani</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoFlavours Sandwich: Chocolate Toast</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoRudra Café: Breadcrumbs</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoVaishali: Cold Bournvita</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoKayani Bakery: Shrewsbury Cookies</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoYewale Amruttulya: Tea</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoCafe Goodluck: Bun Maska</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoFalahaar: Jamun Shot</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoYashwant Dabeli</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoDurga Cafe: Cold Coffee and Anda Bhurji</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoSukanta: Thali</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoKadhai: Jalebi</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoIndorilaal: Kachori</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoKohinoor Restaurant: Omelette and Chai</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoKalyan Bhel: Pani Puri</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoThe Place: Sizzler</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoJain Boarding: Lunch Menu</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoBhadait Misal: Misal</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoMasaledar Biryani House: Biryani</t>
-  </si>
-  <si>
-    <t>Shiv Kailash Dairy: Special DoodhtoShiv Kailash Dairy: Special Doodh</t>
+    <t>HOME to HOME</t>
+  </si>
+  <si>
+    <t>HOME to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>HOME to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>HOME to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>HOME to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>HOME to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>HOME to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>HOME to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>HOME to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>HOME to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>HOME to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>HOME to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>HOME to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>HOME to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>HOME to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>HOME to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>HOME to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>HOME to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>HOME to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>HOME to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>HOME to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>HOME to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>HOME to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>HOME to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to HOME</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Garden Vada Pav to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to HOME</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Santosh Bakery: Pattice to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to HOME</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Chitale Bandhu: Bakarwadi to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to HOME</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Sujata Mastani to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to HOME</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Flavours Sandwich: Chocolate Toast to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to HOME</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Rudra Café: Breadcrumbs to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to HOME</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Vaishali: Cold Bournvita to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to HOME</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Kayani Bakery: Shrewsbury Cookies to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to HOME</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Yewale Amruttulya: Tea to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to HOME</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Cafe Goodluck: Bun Maska to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to HOME</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Falahaar: Jamun Shot to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to HOME</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Yashwant Dabeli to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to HOME</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Durga Cafe: Cold Coffee and Anda Bhurji to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to HOME</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Sukanta: Thali to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to HOME</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Kadhai: Jalebi to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to HOME</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Indorilaal: Kachori to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to HOME</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Kohinoor Restaurant: Omelette and Chai to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to HOME</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Kalyan Bhel: Pani Puri to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to HOME</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>The Place: Sizzler to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to HOME</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Jain Boarding: Lunch Menu to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to HOME</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Bhadait Misal: Misal to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to HOME</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Masaledar Biryani House: Biryani to Shiv Kailash Dairy: Special Doodh</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to HOME</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Garden Vada Pav</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Santosh Bakery: Pattice</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Chitale Bandhu: Bakarwadi</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Sujata Mastani</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Flavours Sandwich: Chocolate Toast</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Rudra Café: Breadcrumbs</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Vaishali: Cold Bournvita</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Kayani Bakery: Shrewsbury Cookies</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Yewale Amruttulya: Tea</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Cafe Goodluck: Bun Maska</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Falahaar: Jamun Shot</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Yashwant Dabeli</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Durga Cafe: Cold Coffee and Anda Bhurji</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Sukanta: Thali</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Kadhai: Jalebi</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Indorilaal: Kachori</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Kohinoor Restaurant: Omelette and Chai</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Kalyan Bhel: Pani Puri</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to The Place: Sizzler</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Jain Boarding: Lunch Menu</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Bhadait Misal: Misal</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Masaledar Biryani House: Biryani</t>
+  </si>
+  <si>
+    <t>Shiv Kailash Dairy: Special Doodh to Shiv Kailash Dairy: Special Doodh</t>
   </si>
 </sst>
 </file>
@@ -1990,7 +1990,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2027,7 +2027,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2050,44 +2050,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -2117,12 +2117,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -2161,218 +2161,158 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet 1"/>
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1"/>
-    <col min="2" max="2" width="23.875" customWidth="1"/>
-    <col min="3" max="3" width="25.625" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" customWidth="1"/>
+    <col min="3" max="3" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2650,7 +2590,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2855,7 +2795,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3060,7 +3000,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3265,7 +3205,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3470,7 +3413,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3675,7 +3618,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3880,7 +3823,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4085,7 +4028,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4290,7 +4233,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4495,7 +4438,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4698,11 +4641,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.375" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -4908,7 +4851,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5113,7 +5056,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5318,7 +5261,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5521,9 +5464,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5728,7 +5674,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="64.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5933,7 +5882,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="80.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -6138,7 +6090,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="64.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -6343,7 +6298,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="62.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -6548,7 +6506,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="61.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -6753,7 +6714,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -6958,7 +6919,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7163,7 +7124,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7368,7 +7329,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>